<commit_message>
Add header validation to bulk uplods
</commit_message>
<xml_diff>
--- a/tests/files/bulk_curation_upload_bad.xlsx
+++ b/tests/files/bulk_curation_upload_bad.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jward3/projects/clingen/tests/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yugen/code/gene-tracker/tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{85B06B87-6E34-D345-B244-833EFE59BA17}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C233DAB-F62D-8547-9526-8691FFD95C8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{86F797EF-5C7F-3A42-85FA-E5257E13070D}"/>
   </bookViews>
@@ -247,9 +247,6 @@
     <t>PMID 10</t>
   </si>
   <si>
-    <t>Uploaded Date</t>
-  </si>
-  <si>
     <t>Precuration Date</t>
   </si>
   <si>
@@ -263,6 +260,9 @@
   </si>
   <si>
     <t>Curation Approved Date</t>
+  </si>
+  <si>
+    <t>Date Uploaded</t>
   </si>
 </sst>
 </file>
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7E3D26-773C-0343-9D4F-0C8AA45D4AC9}">
   <dimension ref="A1:AJ254"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -862,22 +862,22 @@
         <v>72</v>
       </c>
       <c r="AE1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF1" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AG1" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AH1" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AI1" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="AJ1" s="12" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updates for improved dev setup.
</commit_message>
<xml_diff>
--- a/tests/files/bulk_curation_upload_bad.xlsx
+++ b/tests/files/bulk_curation_upload_bad.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yugen/code/gene-tracker/tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C233DAB-F62D-8547-9526-8691FFD95C8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902455C9-12A9-E548-8966-EE6D2BB46163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{86F797EF-5C7F-3A42-85FA-E5257E13070D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17540" xr2:uid="{86F797EF-5C7F-3A42-85FA-E5257E13070D}"/>
   </bookViews>
   <sheets>
     <sheet name="Curations" sheetId="1" r:id="rId1"/>
     <sheet name="lookups" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -145,9 +156,6 @@
     <t>BRCA1</t>
   </si>
   <si>
-    <t>sirs@unc.edu</t>
-  </si>
-  <si>
     <t>notes on the rationale</t>
   </si>
   <si>
@@ -263,6 +271,9 @@
   </si>
   <si>
     <t>Date Uploaded</t>
+  </si>
+  <si>
+    <t>super.user@example.com</t>
   </si>
 </sst>
 </file>
@@ -745,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7E3D26-773C-0343-9D4F-0C8AA45D4AC9}">
   <dimension ref="A1:AJ254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,103 +792,103 @@
         <v>37</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>53</v>
       </c>
       <c r="N1" s="12" t="s">
         <v>35</v>
       </c>
       <c r="O1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="T1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AD1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AE1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF1" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="AE1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AG1" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AH1" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AI1" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>76</v>
-      </c>
-      <c r="AJ1" s="12" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
@@ -885,7 +896,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -900,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z2" s="9"/>
       <c r="AA2" s="9"/>
@@ -917,17 +928,17 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="10"/>
       <c r="O3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P3" t="s">
         <v>0</v>
@@ -936,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="T3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="9"/>
       <c r="AA3" s="9"/>
@@ -955,26 +966,26 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="10"/>
       <c r="O4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q4" t="s">
         <v>1</v>
       </c>
       <c r="T4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z4" s="9"/>
       <c r="AA4" s="9"/>
@@ -993,7 +1004,7 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -1010,7 +1021,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -1025,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="T6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z6" s="9"/>
       <c r="AA6" s="9"/>
@@ -2134,10 +2145,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{A80EC79B-2F5D-8F44-B6B0-940454424882}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{B36354CF-ECBE-8846-A16E-88DC87860498}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{DF605ACA-064E-9F45-AC4B-73E8A56122D1}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{42F85008-A4C4-9C42-8EB0-F4BF2250B21C}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{7D876844-BB32-5A49-B7C2-8729D7760657}"/>
+    <hyperlink ref="B3:B6" r:id="rId2" display="super.user@example.com" xr:uid="{A3995F7F-6D1C-AB47-B20C-702156D2B22C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>